<commit_message>
adding data to graphics
</commit_message>
<xml_diff>
--- a/articles/aosd_2014/graficos.xlsx
+++ b/articles/aosd_2014/graficos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21160" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6640" yWindow="21160" windowWidth="25600" windowHeight="14780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Size Distribution" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
   <si>
     <t>Static</t>
   </si>
@@ -271,6 +271,12 @@
   <si>
     <t>Dyanmic Typing Usage</t>
   </si>
+  <si>
+    <t>Total Static</t>
+  </si>
+  <si>
+    <t>Total Dynamic</t>
+  </si>
 </sst>
 </file>
 
@@ -333,11 +339,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,7 +428,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -422,6 +450,17 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -443,6 +482,17 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -8246,16 +8296,16 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Method Return</c:v>
+                  <c:v>Constructor Parameter</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Method Parameter</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Constructor Parameter</c:v>
+                  <c:v>Field</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Field</c:v>
+                  <c:v>Method Return</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Local Variable</c:v>
@@ -8270,19 +8320,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>71.16126285053835</c:v>
+                  <c:v>91.73578440703777</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.2131047634026</c:v>
+                  <c:v>81.7578163631483</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91.5145693243676</c:v>
+                  <c:v>78.50402761795166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78.50402761795166</c:v>
+                  <c:v>67.7496649724876</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.2353816509911</c:v>
+                  <c:v>29.20195634021233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8327,16 +8377,16 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Method Return</c:v>
+                  <c:v>Constructor Parameter</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Method Parameter</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Constructor Parameter</c:v>
+                  <c:v>Field</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Field</c:v>
+                  <c:v>Method Return</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Local Variable</c:v>
@@ -8351,19 +8401,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>28.83873714946165</c:v>
+                  <c:v>8.264215592962227</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.7868952365974</c:v>
+                  <c:v>18.2421836368517</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.485430675632404</c:v>
+                  <c:v>21.49597238204833</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.49597238204833</c:v>
+                  <c:v>32.2503350275124</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.7646183490089</c:v>
+                  <c:v>70.79804365978766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8629,7 +8679,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>70.50645883336479</c:v>
+                  <c:v>67.25603337362081</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>64.43768996960486</c:v>
@@ -8641,19 +8691,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>80.97043389814835</c:v>
+                  <c:v>82.37878671086102</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.0">
-                  <c:v>70.14869188782232</c:v>
+                  <c:v>67.17342342342343</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.0">
-                  <c:v>89.23747276688454</c:v>
+                  <c:v>86.63282571912013</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.0">
-                  <c:v>91.69093851132686</c:v>
+                  <c:v>91.79607543462242</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0">
                   <c:v>63.01369863013699</c:v>
@@ -8759,7 +8809,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>29.4935411666352</c:v>
+                  <c:v>32.7439666263792</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>35.56231003039513</c:v>
@@ -8771,19 +8821,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>19.02956610185164</c:v>
+                  <c:v>17.62121328913898</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.0">
-                  <c:v>29.85130811217768</c:v>
+                  <c:v>32.82657657657658</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.0">
-                  <c:v>10.76252723311547</c:v>
+                  <c:v>13.36717428087987</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.0">
-                  <c:v>8.309061488673139</c:v>
+                  <c:v>8.203924565377582</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0">
                   <c:v>36.98630136986301</c:v>
@@ -9018,7 +9068,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>70.50645883336479</c:v>
+                  <c:v>67.25603337362081</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>64.43768996960486</c:v>
@@ -9087,7 +9137,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>29.4935411666352</c:v>
+                  <c:v>32.7439666263792</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>35.56231003039513</c:v>
@@ -9335,13 +9385,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>80.97043389814835</c:v>
+                  <c:v>82.37878671086102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70.14869188782232</c:v>
+                  <c:v>67.17342342342343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.23747276688454</c:v>
+                  <c:v>86.63282571912013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9404,13 +9454,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19.02956610185164</c:v>
+                  <c:v>17.62121328913898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.85130811217768</c:v>
+                  <c:v>32.82657657657658</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.76252723311547</c:v>
+                  <c:v>13.36717428087987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9969,7 +10019,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>91.69093851132686</c:v>
+                  <c:v>91.79607543462242</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>63.01369863013699</c:v>
@@ -10038,7 +10088,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.309061488673139</c:v>
+                  <c:v>8.203924565377582</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>36.98630136986301</c:v>
@@ -25544,7 +25594,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -25574,29 +25624,29 @@
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C2">
-        <v>58491</v>
+        <v>33734</v>
       </c>
       <c r="D2">
-        <v>23704</v>
+        <v>3039</v>
       </c>
       <c r="E2">
         <f>C2+D2</f>
-        <v>82195</v>
+        <v>36773</v>
       </c>
       <c r="F2" t="str">
-        <f>A2</f>
-        <v>Method Return</v>
+        <f t="shared" ref="F2:F6" si="0">A2</f>
+        <v>Constructor Parameter</v>
       </c>
       <c r="G2" s="6">
-        <f>100*C2/E2</f>
-        <v>71.16126285053835</v>
+        <f t="shared" ref="G2:G6" si="1">100*C2/E2</f>
+        <v>91.735784407037769</v>
       </c>
       <c r="H2" s="6">
-        <f>100*D2/E2</f>
-        <v>28.838737149461647</v>
+        <f t="shared" ref="H2:H6" si="2">100*D2/E2</f>
+        <v>8.264215592962227</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1">
@@ -25604,80 +25654,80 @@
         <v>71</v>
       </c>
       <c r="C3">
-        <v>40802</v>
+        <v>57869</v>
       </c>
       <c r="D3">
-        <v>10065</v>
+        <v>12912</v>
       </c>
       <c r="E3">
         <f>C3+D3</f>
-        <v>50867</v>
+        <v>70781</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F6" si="0">A3</f>
+        <f>A3</f>
         <v>Method Parameter</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G6" si="1">100*C3/E3</f>
-        <v>80.213104763402598</v>
+        <f>100*C3/E3</f>
+        <v>81.757816363148308</v>
       </c>
       <c r="H3" s="6">
-        <f t="shared" ref="H3:H6" si="2">100*D3/E3</f>
-        <v>19.786895236597402</v>
+        <f>100*D3/E3</f>
+        <v>18.242183636851699</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C4">
-        <v>11432</v>
+        <v>6822</v>
       </c>
       <c r="D4">
-        <v>1060</v>
+        <v>1868</v>
       </c>
       <c r="E4">
         <f>C4+D4</f>
-        <v>12492</v>
+        <v>8690</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>Constructor Parameter</v>
+        <v>Field</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" si="1"/>
-        <v>91.514569324367599</v>
+        <v>78.504027617951664</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" si="2"/>
-        <v>8.4854306756324043</v>
+        <v>21.495972382048333</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5">
-        <v>6822</v>
+        <v>109705</v>
       </c>
       <c r="D5">
-        <v>1868</v>
+        <v>52222</v>
       </c>
       <c r="E5">
         <f>C5+D5</f>
-        <v>8690</v>
+        <v>161927</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>Field</v>
+        <f>A5</f>
+        <v>Method Return</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="1"/>
-        <v>78.504027617951664</v>
+        <f>100*C5/E5</f>
+        <v>67.749664972487608</v>
       </c>
       <c r="H5" s="6">
-        <f t="shared" si="2"/>
-        <v>21.495972382048333</v>
+        <f>100*D5/E5</f>
+        <v>32.250335027512399</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1">
@@ -25685,14 +25735,14 @@
         <v>74</v>
       </c>
       <c r="C6">
-        <v>37987</v>
+        <v>39168</v>
       </c>
       <c r="D6">
-        <v>66847</v>
+        <v>94960</v>
       </c>
       <c r="E6">
         <f>C6+D6</f>
-        <v>104834</v>
+        <v>134128</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -25700,11 +25750,11 @@
       </c>
       <c r="G6" s="6">
         <f t="shared" si="1"/>
-        <v>36.235381650991094</v>
+        <v>29.201956340212334</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="2"/>
-        <v>63.764618349008906</v>
+        <v>70.798043659787666</v>
       </c>
     </row>
   </sheetData>
@@ -25720,10 +25770,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -25734,7 +25784,7 @@
     <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:10" ht="12.75" customHeight="1">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -25750,20 +25800,26 @@
       <c r="H1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" customHeight="1">
       <c r="B2" t="s">
         <v>75</v>
       </c>
       <c r="C2">
-        <v>52289</v>
+        <v>103503</v>
       </c>
       <c r="D2">
-        <v>21873</v>
+        <v>50391</v>
       </c>
       <c r="E2">
         <f>C2+D2</f>
-        <v>74162</v>
+        <v>153894</v>
       </c>
       <c r="F2" t="str">
         <f>B2</f>
@@ -25771,14 +25827,22 @@
       </c>
       <c r="G2" s="5">
         <f>C2/E2*100</f>
-        <v>70.506458833364789</v>
+        <v>67.256033373620809</v>
       </c>
       <c r="H2" s="5">
         <f>100*D2/E2</f>
-        <v>29.493541166635204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+        <v>32.743966626379198</v>
+      </c>
+      <c r="I2">
+        <f>SUM(C2:C4)</f>
+        <v>109705</v>
+      </c>
+      <c r="J2">
+        <f>SUM(D2:D4)</f>
+        <v>52222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -25808,7 +25872,7 @@
         <v>35.562310030395139</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -25835,7 +25899,7 @@
         <v>8.25346112886049</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1">
       <c r="G5" t="str">
         <f>G1</f>
         <v>Statically Typed (%)</v>
@@ -25845,19 +25909,19 @@
         <v>Dynamically Typed (%)</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1">
       <c r="B6" t="s">
         <v>75</v>
       </c>
       <c r="C6">
-        <v>35027</v>
+        <v>53435</v>
       </c>
       <c r="D6">
-        <v>8232</v>
+        <v>11430</v>
       </c>
       <c r="E6">
         <f>C6+D6</f>
-        <v>43259</v>
+        <v>64865</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -25865,14 +25929,22 @@
       </c>
       <c r="G6" s="6">
         <f>100*C6/E6</f>
-        <v>80.970433898148357</v>
+        <v>82.378786710861021</v>
       </c>
       <c r="H6" s="6">
         <f>100*D6/E6</f>
-        <v>19.029566101851639</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+        <v>17.621213289138982</v>
+      </c>
+      <c r="I6">
+        <f>SUM(C6:C8)</f>
+        <v>57869</v>
+      </c>
+      <c r="J6">
+        <f>SUM(D6:D8)</f>
+        <v>12912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -25880,14 +25952,14 @@
         <v>76</v>
       </c>
       <c r="C7">
-        <v>3727</v>
+        <v>2386</v>
       </c>
       <c r="D7">
-        <v>1586</v>
+        <v>1166</v>
       </c>
       <c r="E7">
         <f>C7+D7</f>
-        <v>5313</v>
+        <v>3552</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -25895,14 +25967,14 @@
       </c>
       <c r="G7" s="6">
         <f t="shared" ref="G7:G8" si="3">100*C7/E7</f>
-        <v>70.148691887822324</v>
+        <v>67.173423423423429</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" ref="H7:H8" si="4">100*D7/E7</f>
-        <v>29.851308112177676</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+        <v>32.826576576576578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" customHeight="1">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -25910,11 +25982,11 @@
         <v>2048</v>
       </c>
       <c r="D8">
-        <v>247</v>
+        <v>316</v>
       </c>
       <c r="E8">
         <f>C8+D8</f>
-        <v>2295</v>
+        <v>2364</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -25922,14 +25994,14 @@
       </c>
       <c r="G8" s="6">
         <f t="shared" si="3"/>
-        <v>89.237472766884537</v>
+        <v>86.632825719120135</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="4"/>
-        <v>10.762527233115469</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+        <v>13.367174280879865</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" customHeight="1">
       <c r="G9" t="str">
         <f>G5</f>
         <v>Statically Typed (%)</v>
@@ -25939,19 +26011,19 @@
         <v>Dynamically Typed (%)</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1">
       <c r="B10" t="s">
         <v>75</v>
       </c>
       <c r="C10">
-        <v>11333</v>
+        <v>33635</v>
       </c>
       <c r="D10">
-        <v>1027</v>
+        <v>3006</v>
       </c>
       <c r="E10">
         <f>C10+D10</f>
-        <v>12360</v>
+        <v>36641</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -25959,14 +26031,22 @@
       </c>
       <c r="G10" s="6">
         <f>100*C10/E10</f>
-        <v>91.690938511326863</v>
+        <v>91.796075434622423</v>
       </c>
       <c r="H10" s="6">
         <f>100*D10/E10</f>
-        <v>8.3090614886731391</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+        <v>8.2039245653775819</v>
+      </c>
+      <c r="I10">
+        <f>SUM(C10:C12)</f>
+        <v>33734</v>
+      </c>
+      <c r="J10">
+        <f>SUM(D10:D12)</f>
+        <v>3039</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -25996,7 +26076,7 @@
         <v>36.986301369863014</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -26023,7 +26103,7 @@
         <v>10.169491525423728</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
+    <row r="13" spans="1:10" ht="12.75" customHeight="1">
       <c r="G13" t="str">
         <f>G9</f>
         <v>Statically Typed (%)</v>
@@ -26033,7 +26113,7 @@
         <v>Dynamically Typed (%)</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
+    <row r="14" spans="1:10" ht="12.75" customHeight="1">
       <c r="B14" t="s">
         <v>75</v>
       </c>
@@ -26059,8 +26139,16 @@
         <f>100*D14/E14</f>
         <v>11.232980332829047</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1">
+      <c r="I14">
+        <f>SUM(C14:C16)</f>
+        <v>6822</v>
+      </c>
+      <c r="J14">
+        <f>SUM(D14:D16)</f>
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -26090,7 +26178,7 @@
         <v>27.562127746970631</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -26202,7 +26290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>

</xml_diff>